<commit_message>
Changed CaseField ID to be different
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Invalid_ChangeOrganisationRequest_Defined_Twice.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Invalid_ChangeOrganisationRequest_Defined_Twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A25A8D-076B-6647-A8A2-B2F2FB36605A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D535BF-0549-9F4F-AC24-9E29D977FE9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="900" windowWidth="30680" windowHeight="19860" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34102,7 +34102,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{6F3568F8-75DC-994A-9CD6-5C91B079C7DC}">
           <x14:formula1>
-            <xm:f>'/Users/hmcts/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\dev\Documents\Definition Files\[RDM-8509.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/hmcts/Library/Containers/com.microsoft.Excel/Data/Documents/Users\dev\Documents\Definition Files\[RDM-8509.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
@@ -48229,8 +48229,8 @@
   <dimension ref="A1:IO186"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -49674,7 +49674,7 @@
         <v>82</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E45" s="57" t="s">
         <v>254</v>

</xml_diff>